<commit_message>
main page is done
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">en</t>
   </si>
   <si>
-    <t xml:space="preserve">jp</t>
+    <t xml:space="preserve">ja</t>
   </si>
   <si>
     <t xml:space="preserve">de</t>
@@ -203,6 +203,232 @@
   </si>
   <si>
     <t xml:space="preserve">notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital_skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programming languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmiersprache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprachen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">japanese_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日本語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">japanese_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native</t>
+  </si>
+  <si>
+    <t xml:space="preserve">母語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">英語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Englisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily use for Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ビジネス利用</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Täglich für Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">german_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">German</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ドイツ語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deutsch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">german_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Around B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ungefär B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">french_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">フランス語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Französisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">french_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persian_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ペルシア語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persian_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausbildungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">master_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.E. in Computational Linguistics</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">修士 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">計算機言語学</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">master_school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nara Institute of science and Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈良先端科学技術大学院大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bachelor_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.A. in Foreign Studies&amp;nbsp;(Persian studies)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">学士 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">外国語</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B.A. in Foreign Studies (Persian studies)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bachelor_school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osaka University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大阪大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">berufliche Erfahrungen</t>
   </si>
 </sst>
 </file>
@@ -320,15 +546,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
@@ -496,6 +723,312 @@
         <v>37</v>
       </c>
       <c r="C10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
correction on spell error
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -96,13 +96,13 @@
     <t xml:space="preserve">自然言語処理技術・機械学習の研究活動，または，これらの技術を使ったシステム開発を得意にしています。</t>
   </si>
   <si>
-    <t xml:space="preserve">Ziemlich Spezialisierung auf NLP (Natural Language Processing) mit Kentnisse des linguistischen Fachs.</t>
+    <t xml:space="preserve">Ziemlich Spezialisierung auf NLP (Natural Language Processing) mit Kenntnisse der Linguistik.</t>
   </si>
   <si>
     <t xml:space="preserve">work_experience</t>
   </si>
   <si>
-    <t xml:space="preserve">For work experience, I have experience in data analytics from log data for the social game, machine learning techniques for NLP solutions, such as text summarization, document clustering/classification, information retrieval etc. Not only data analysis but also I have experience in system development for data analytics. For that, I am able to consider hardware, DB specification, deployment, and operations with using Jenkins, Docker etc. In the point of system admin, I have experience of business system migration for a small team. Thus, I am able to make IT/development plans with considering business roadmaps.</t>
+    <t xml:space="preserve">For work experience, I have experience in data analytics from log data for the social game, machine learning techniques for NLP solutions, such as text summarization, document clustering/classification, information retrieval, etc. Not only data analysis but also I have experience in system development for data analytics. For that, I can consider hardware, DB specification, deployment, and operations using Jenkins, Docker, etc. In the point of system admin, I have experience in business system migration for a small team. Thus, I can make IT/development plans by considering business roadmaps.</t>
   </si>
   <si>
     <t xml:space="preserve">データ処理、データ解析、データ解析システムの設計、データ解析システムのための環境構築などの経験があります。一度限りの解析用プログラムの開発だけでなく、ハードウェアの選定からデータベースの設計、デプロイメント設計まで含めた安定的に運用できる解析システムの構築までが可能です。これまでにレポートシステム、テキストクラスタリングシステム、情報抽出システムの開発を手がけてきました。</t>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">work_environment</t>
   </si>
   <si>
-    <t xml:space="preserve">I have +3 years work experience in an international work environment. In such environment, I am able to communicate with other members with English.</t>
+    <t xml:space="preserve">I have +3 years of work experience in an international work environment. In such an environment, I can communicate with other members with English.</t>
   </si>
   <si>
     <r>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">research_preference</t>
   </si>
   <si>
-    <t xml:space="preserve">For research perspective, I am interested in information extraction/information retrieval from the text. This is because I have worked for 3.5 years on projects to extract business useful information from the text which is posted to an opinion-platform called "Fuman Kaitori" so that I feel technical limitations of existing NLP methods.</t>
+    <t xml:space="preserve">For a research perspective, I am interested in information extraction/information retrieval from the text. This is because I have worked for 3.5 years on projects to extract business useful information from the text which is posted to an opinion-platform called "Fuman Kaitori" so that I feel technical limitations of existing NLP methods.</t>
   </si>
   <si>
     <t xml:space="preserve">システム開発だけでなく、企業ブランディングのための研究活動計画の立案、研究連携活動の経験、対外論文発表もあります。</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">research_experience</t>
   </si>
   <si>
-    <t xml:space="preserve">To this day, I had research experience in Auto-Error-Correction of English text, document classification for folk narratives and Rule-based translation of Sign language from Japanese text.</t>
+    <t xml:space="preserve">To this day, I had research experience in Auto-Error-Correction of English text, document classification for folk narratives, and Rule-based translation of Sign language from Japanese text.</t>
   </si>
   <si>
     <t xml:space="preserve">研究面では，自然言語処理技術，特に計算機を使った物語・小説の構造化という分野に興味があります。これまでに取り組んできた内容には，自然言語処理技術を利用した英文誤りの自動訂正，自然言語文で書かれた文章を手話で表現する研究があります。</t>
@@ -223,6 +223,9 @@
     <t xml:space="preserve">programming languages</t>
   </si>
   <si>
+    <t xml:space="preserve">プログラミング言語</t>
+  </si>
+  <si>
     <t xml:space="preserve">Programmiersprache</t>
   </si>
   <si>
@@ -232,6 +235,9 @@
     <t xml:space="preserve">Languages</t>
   </si>
   <si>
+    <t xml:space="preserve">語学</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprachen</t>
   </si>
   <si>
@@ -346,6 +352,9 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
+    <t xml:space="preserve">学歴</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ausbildungen</t>
   </si>
   <si>
@@ -438,6 +447,9 @@
   </si>
   <si>
     <t xml:space="preserve">Work experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">職歴</t>
   </si>
   <si>
     <t xml:space="preserve">berufliche Erfahrungen</t>
@@ -450,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -483,6 +495,11 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -527,7 +544,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +559,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -563,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -641,7 +666,7 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -749,283 +774,283 @@
       <c r="C11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>40</v>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,13 +1061,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>